<commit_message>
Proj1 and Proj2 submission done.
</commit_message>
<xml_diff>
--- a/proj1/marksheets/1401CB01.xlsx
+++ b/proj1/marksheets/1401CB01.xlsx
@@ -636,7 +636,7 @@
         </is>
       </c>
       <c r="B11" s="7" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C11" s="8" t="n">
         <v>-2</v>
@@ -653,7 +653,7 @@
         </is>
       </c>
       <c r="B12" s="7" t="n">
-        <v>56</v>
+        <v>70</v>
       </c>
       <c r="C12" s="8" t="n">
         <v>28</v>
@@ -661,7 +661,7 @@
       <c r="D12" s="5" t="n"/>
       <c r="E12" s="9" t="inlineStr">
         <is>
-          <t>28/112</t>
+          <t>42/140</t>
         </is>
       </c>
     </row>

</xml_diff>